<commit_message>
Fixed GitHub issue #1 typo Verity should be Verify in CODE-009-LEVEL-1
</commit_message>
<xml_diff>
--- a/v1/DevSecOps-VerificationStandard-v1.xlsx
+++ b/v1/DevSecOps-VerificationStandard-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yudhi\Desktop\DSOVS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\www-project-devsecops-verification-standard\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954E3B8E-2507-4D34-8010-8388466B1328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8ECA7F-C09F-4BA6-ABF5-A2947EFA4D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8830" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28420" yWindow="-20560" windowWidth="28800" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -1249,9 +1249,6 @@
     <t>Direct use of public repositories for third-party dependencies and libraries.</t>
   </si>
   <si>
-    <t>Verity implementation of a private repository to manage third-party dependencies and libraries.</t>
-  </si>
-  <si>
     <t>Verify that only verified third-party dependencies and libraries can be used by the application.</t>
   </si>
   <si>
@@ -1334,6 +1331,9 @@
   </si>
   <si>
     <t>No package/code signing process defined.</t>
+  </si>
+  <si>
+    <t>Verify implementation of a private repository to manage third-party dependencies and libraries.</t>
   </si>
 </sst>
 </file>
@@ -2016,17 +2016,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2034,56 +2040,11 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2097,10 +2058,49 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4922,8 +4922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDAC9A0-62CC-4A20-8692-B712C8E85C25}">
   <dimension ref="A1:C197"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B166" sqref="B166"/>
+    <sheetView topLeftCell="A76" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5309,7 +5309,7 @@
         <v>202</v>
       </c>
       <c r="B47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -5605,7 +5605,7 @@
         <v>239</v>
       </c>
       <c r="B84" s="65" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -5733,7 +5733,7 @@
         <v>255</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>402</v>
+        <v>430</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -5741,7 +5741,7 @@
         <v>256</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -5749,7 +5749,7 @@
         <v>257</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -5765,7 +5765,7 @@
         <v>259</v>
       </c>
       <c r="B104" s="65" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -5805,7 +5805,7 @@
         <v>264</v>
       </c>
       <c r="B109" s="65" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -5845,7 +5845,7 @@
         <v>269</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -5885,7 +5885,7 @@
         <v>274</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -5925,7 +5925,7 @@
         <v>279</v>
       </c>
       <c r="B124" s="65" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -5965,7 +5965,7 @@
         <v>284</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -6005,7 +6005,7 @@
         <v>289</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -6045,7 +6045,7 @@
         <v>294</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -6085,7 +6085,7 @@
         <v>299</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -6117,7 +6117,7 @@
         <v>303</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -6125,7 +6125,7 @@
         <v>304</v>
       </c>
       <c r="B149" s="65" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
@@ -6141,7 +6141,7 @@
         <v>306</v>
       </c>
       <c r="B151" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -6165,7 +6165,7 @@
         <v>309</v>
       </c>
       <c r="B154" s="65" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -6205,7 +6205,7 @@
         <v>314</v>
       </c>
       <c r="B159" s="65" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
@@ -6245,7 +6245,7 @@
         <v>319</v>
       </c>
       <c r="B164" s="65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
@@ -6277,7 +6277,7 @@
         <v>323</v>
       </c>
       <c r="B168" s="65" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -6285,7 +6285,7 @@
         <v>324</v>
       </c>
       <c r="B169" s="65" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
@@ -6317,7 +6317,7 @@
         <v>328</v>
       </c>
       <c r="B173" s="65" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -6325,7 +6325,7 @@
         <v>329</v>
       </c>
       <c r="B174" s="65" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
@@ -6357,7 +6357,7 @@
         <v>333</v>
       </c>
       <c r="B178" s="65" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -6365,7 +6365,7 @@
         <v>334</v>
       </c>
       <c r="B179" s="65" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -6397,7 +6397,7 @@
         <v>338</v>
       </c>
       <c r="B183" s="65" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
@@ -6405,7 +6405,7 @@
         <v>339</v>
       </c>
       <c r="B184" s="65" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
@@ -6445,7 +6445,7 @@
         <v>344</v>
       </c>
       <c r="B189" s="65" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
@@ -6485,7 +6485,7 @@
         <v>349</v>
       </c>
       <c r="B194" s="65" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
@@ -6527,7 +6527,7 @@
   <dimension ref="A1:K1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6569,10 +6569,10 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6584,10 +6584,10 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="78" t="str">
+      <c r="B3" s="74" t="str">
         <f>VLOOKUP(CONCATENATE($A3, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Risk Assessment</v>
       </c>
@@ -6614,8 +6614,8 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="79"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -6627,10 +6627,10 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="78" t="str">
+      <c r="B5" s="74" t="str">
         <f>VLOOKUP(CONCATENATE($A5, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Training</v>
       </c>
@@ -6657,8 +6657,8 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -6670,10 +6670,10 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="78" t="str">
+      <c r="B7" s="74" t="str">
         <f>VLOOKUP(CONCATENATE($A7, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Champion</v>
       </c>
@@ -6700,8 +6700,8 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
@@ -6713,10 +6713,10 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="78" t="str">
+      <c r="B9" s="74" t="str">
         <f>VLOOKUP(CONCATENATE($A9, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Reporting</v>
       </c>
@@ -6743,8 +6743,8 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
@@ -6769,10 +6769,10 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -6784,10 +6784,10 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="89" t="str">
+      <c r="B13" s="76" t="str">
         <f>VLOOKUP(CONCATENATE($A13, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Policy and Regulatory Compliance</v>
       </c>
@@ -6814,8 +6814,8 @@
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
-      <c r="B14" s="90"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="11"/>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
@@ -6827,10 +6827,10 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="89" t="str">
+      <c r="B15" s="76" t="str">
         <f>VLOOKUP(CONCATENATE($A15, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Requirements and Standards</v>
       </c>
@@ -6857,8 +6857,8 @@
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
-      <c r="B16" s="90"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="6"/>
@@ -6870,10 +6870,10 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="89" t="str">
+      <c r="B17" s="76" t="str">
         <f>VLOOKUP(CONCATENATE($A17, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security User Stories and Acceptance Criterias</v>
       </c>
@@ -6900,8 +6900,8 @@
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="90"/>
-      <c r="B18" s="90"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
@@ -6913,10 +6913,10 @@
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="89" t="str">
+      <c r="B19" s="76" t="str">
         <f>VLOOKUP(CONCATENATE($A19, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Issues Tracking</v>
       </c>
@@ -6943,8 +6943,8 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="90"/>
-      <c r="B20" s="90"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
@@ -6969,10 +6969,10 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -6984,10 +6984,10 @@
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="58.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="86" t="s">
+      <c r="A23" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="86" t="str">
+      <c r="B23" s="80" t="str">
         <f>VLOOKUP(CONCATENATE($A23, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Architecture Design Reviews</v>
       </c>
@@ -7014,8 +7014,8 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" s="6"/>
@@ -7057,8 +7057,8 @@
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="6"/>
@@ -7083,10 +7083,10 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84" t="s">
+      <c r="A28" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="85"/>
+      <c r="B28" s="92"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -7098,10 +7098,10 @@
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="68" t="str">
+      <c r="B29" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A29, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secure Development Environment</v>
       </c>
@@ -7128,8 +7128,8 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="69"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="6"/>
@@ -7141,10 +7141,10 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="68" t="str">
+      <c r="B31" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A31, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Hardcoded Secrets Detection</v>
       </c>
@@ -7171,8 +7171,8 @@
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
-      <c r="B32" s="69"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="90"/>
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -7184,10 +7184,10 @@
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="68" t="str">
+      <c r="B33" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A33, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Manual Secure Code Review</v>
       </c>
@@ -7214,8 +7214,8 @@
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="69"/>
+      <c r="A34" s="90"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="7"/>
       <c r="D34" s="16"/>
       <c r="E34" s="6"/>
@@ -7227,10 +7227,10 @@
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="68" t="str">
+      <c r="B35" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A35, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Static Application Security Testing (SAST)</v>
       </c>
@@ -7257,8 +7257,8 @@
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="69"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="90"/>
       <c r="C36" s="7"/>
       <c r="D36" s="6"/>
       <c r="E36" s="16"/>
@@ -7270,10 +7270,10 @@
       <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="68" t="str">
+      <c r="B37" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A37, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Software Composition Analysis (SCA)</v>
       </c>
@@ -7300,8 +7300,8 @@
       <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
-      <c r="B38" s="69"/>
+      <c r="A38" s="90"/>
+      <c r="B38" s="90"/>
       <c r="C38" s="7"/>
       <c r="D38" s="6"/>
       <c r="E38" s="16"/>
@@ -7313,10 +7313,10 @@
       <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="68" t="str">
+      <c r="B39" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A39, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Software License Compliance</v>
       </c>
@@ -7343,8 +7343,8 @@
       <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="69"/>
-      <c r="B40" s="69"/>
+      <c r="A40" s="90"/>
+      <c r="B40" s="90"/>
       <c r="C40" s="7"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -7356,10 +7356,10 @@
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="68" t="s">
+      <c r="A41" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="68" t="str">
+      <c r="B41" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A41, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Inline IDE Secure Code Analysis</v>
       </c>
@@ -7386,8 +7386,8 @@
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="69"/>
-      <c r="B42" s="69"/>
+      <c r="A42" s="90"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="7"/>
       <c r="D42" s="16"/>
       <c r="E42" s="6"/>
@@ -7399,10 +7399,10 @@
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="68" t="str">
+      <c r="B43" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A43, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Container Security Scanning</v>
       </c>
@@ -7429,8 +7429,8 @@
       <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
-      <c r="B44" s="69"/>
+      <c r="A44" s="90"/>
+      <c r="B44" s="90"/>
       <c r="C44" s="7"/>
       <c r="D44" s="6"/>
       <c r="E44" s="16"/>
@@ -7442,10 +7442,10 @@
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="B45" s="68" t="str">
+      <c r="B45" s="89" t="str">
         <f>VLOOKUP(CONCATENATE($A45, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secure Dependency Management</v>
       </c>
@@ -7455,7 +7455,7 @@
       </c>
       <c r="D45" s="15" t="str">
         <f>VLOOKUP(CONCATENATE($A45, "-", D$1),LevelDescription,2,FALSE)</f>
-        <v>Verity implementation of a private repository to manage third-party dependencies and libraries.</v>
+        <v>Verify implementation of a private repository to manage third-party dependencies and libraries.</v>
       </c>
       <c r="E45" s="15" t="str">
         <f>VLOOKUP(CONCATENATE($A45, "-", E$1),LevelDescription,2,FALSE)</f>
@@ -7472,8 +7472,8 @@
       <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="69"/>
-      <c r="B46" s="69"/>
+      <c r="A46" s="90"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="7"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -7498,10 +7498,10 @@
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="81"/>
+      <c r="B48" s="88"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -7513,10 +7513,10 @@
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="66" t="str">
+      <c r="B49" s="68" t="str">
         <f>VLOOKUP(CONCATENATE($A49, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Test Management</v>
       </c>
@@ -7543,8 +7543,8 @@
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="67"/>
-      <c r="B50" s="67"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="69"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
@@ -7556,10 +7556,10 @@
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="66" t="str">
+      <c r="B51" s="68" t="str">
         <f>VLOOKUP(CONCATENATE($A51, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Dynamic Application Security Testing (DAST)</v>
       </c>
@@ -7586,8 +7586,8 @@
       <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="67"/>
-      <c r="B52" s="67"/>
+      <c r="A52" s="69"/>
+      <c r="B52" s="69"/>
       <c r="C52" s="7"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -7599,10 +7599,10 @@
       <c r="K52" s="3"/>
     </row>
     <row r="53" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="66" t="str">
+      <c r="B53" s="68" t="str">
         <f>VLOOKUP(CONCATENATE($A53, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Interactive Application Security Testing (IAST)</v>
       </c>
@@ -7629,8 +7629,8 @@
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="67"/>
-      <c r="B54" s="67"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="69"/>
       <c r="C54" s="7"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -7642,10 +7642,10 @@
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="66" t="str">
+      <c r="B55" s="68" t="str">
         <f>VLOOKUP(CONCATENATE($A55, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Penetration Testing</v>
       </c>
@@ -7672,8 +7672,8 @@
       <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="67"/>
-      <c r="B56" s="67"/>
+      <c r="A56" s="69"/>
+      <c r="B56" s="69"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -7685,10 +7685,10 @@
       <c r="K56" s="3"/>
     </row>
     <row r="57" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="66" t="str">
+      <c r="B57" s="68" t="str">
         <f>VLOOKUP(CONCATENATE($A57, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Test Coverage</v>
       </c>
@@ -7715,8 +7715,8 @@
       <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="67"/>
-      <c r="B58" s="67"/>
+      <c r="A58" s="69"/>
+      <c r="B58" s="69"/>
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
       <c r="E58" s="6"/>
@@ -7741,10 +7741,10 @@
       <c r="K59" s="3"/>
     </row>
     <row r="60" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="94"/>
+      <c r="B60" s="71"/>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
@@ -7756,10 +7756,10 @@
       <c r="K60" s="3"/>
     </row>
     <row r="61" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="72" t="s">
+      <c r="A61" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="72" t="str">
+      <c r="B61" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A61, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Artifact Signing</v>
       </c>
@@ -7786,8 +7786,8 @@
       <c r="K61" s="3"/>
     </row>
     <row r="62" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="73"/>
-      <c r="B62" s="73"/>
+      <c r="A62" s="67"/>
+      <c r="B62" s="67"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="6"/>
@@ -7799,10 +7799,10 @@
       <c r="K62" s="3"/>
     </row>
     <row r="63" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="72" t="s">
+      <c r="A63" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="72" t="str">
+      <c r="B63" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A63, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secure Artifact Management</v>
       </c>
@@ -7829,8 +7829,8 @@
       <c r="K63" s="3"/>
     </row>
     <row r="64" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="73"/>
-      <c r="B64" s="73"/>
+      <c r="A64" s="67"/>
+      <c r="B64" s="67"/>
       <c r="C64" s="7"/>
       <c r="D64" s="16"/>
       <c r="E64" s="6"/>
@@ -7842,10 +7842,10 @@
       <c r="K64" s="3"/>
     </row>
     <row r="65" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="72" t="str">
+      <c r="B65" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A65, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secret Management</v>
       </c>
@@ -7872,8 +7872,8 @@
       <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="73"/>
-      <c r="B66" s="73"/>
+      <c r="A66" s="67"/>
+      <c r="B66" s="67"/>
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
       <c r="E66" s="6"/>
@@ -7885,10 +7885,10 @@
       <c r="K66" s="3"/>
     </row>
     <row r="67" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="72" t="s">
+      <c r="A67" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="72" t="str">
+      <c r="B67" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A67, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secure Configuration</v>
       </c>
@@ -7915,8 +7915,8 @@
       <c r="K67" s="3"/>
     </row>
     <row r="68" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="73"/>
-      <c r="B68" s="73"/>
+      <c r="A68" s="67"/>
+      <c r="B68" s="67"/>
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
       <c r="E68" s="6"/>
@@ -7928,10 +7928,10 @@
       <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="72" t="s">
+      <c r="A69" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="72" t="str">
+      <c r="B69" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A69, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Security Policy Enforcement</v>
       </c>
@@ -7958,8 +7958,8 @@
       <c r="K69" s="3"/>
     </row>
     <row r="70" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="73"/>
-      <c r="B70" s="73"/>
+      <c r="A70" s="67"/>
+      <c r="B70" s="67"/>
       <c r="C70" s="7"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -7971,10 +7971,10 @@
       <c r="K70" s="3"/>
     </row>
     <row r="71" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="72" t="s">
+      <c r="A71" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="72" t="str">
+      <c r="B71" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A71, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Infrastructure-as-Code (IaC) Secure Deployment</v>
       </c>
@@ -8001,8 +8001,8 @@
       <c r="K71" s="3"/>
     </row>
     <row r="72" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="73"/>
-      <c r="B72" s="73"/>
+      <c r="A72" s="67"/>
+      <c r="B72" s="67"/>
       <c r="C72" s="7"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -8014,10 +8014,10 @@
       <c r="K72" s="3"/>
     </row>
     <row r="73" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="72" t="s">
+      <c r="A73" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="72" t="str">
+      <c r="B73" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A73, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Compliance Scanning</v>
       </c>
@@ -8044,8 +8044,8 @@
       <c r="K73" s="3"/>
     </row>
     <row r="74" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="73"/>
-      <c r="B74" s="73"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="67"/>
       <c r="C74" s="7"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -8057,10 +8057,10 @@
       <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="72" t="s">
+      <c r="A75" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="72" t="str">
+      <c r="B75" s="66" t="str">
         <f>VLOOKUP(CONCATENATE($A75, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Secure Release Management</v>
       </c>
@@ -8087,8 +8087,8 @@
       <c r="K75" s="3"/>
     </row>
     <row r="76" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="73"/>
-      <c r="B76" s="73"/>
+      <c r="A76" s="67"/>
+      <c r="B76" s="67"/>
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
       <c r="E76" s="6"/>
@@ -8113,10 +8113,10 @@
       <c r="K77" s="3"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="74" t="s">
+      <c r="A78" s="93" t="s">
         <v>147</v>
       </c>
-      <c r="B78" s="75"/>
+      <c r="B78" s="94"/>
       <c r="C78" s="21"/>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
@@ -8128,10 +8128,10 @@
       <c r="K78" s="3"/>
     </row>
     <row r="79" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="70" t="s">
+      <c r="A79" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="70" t="str">
+      <c r="B79" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A79, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Environment Hardening</v>
       </c>
@@ -8158,8 +8158,8 @@
       <c r="K79" s="3"/>
     </row>
     <row r="80" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="71"/>
-      <c r="B80" s="71"/>
+      <c r="A80" s="73"/>
+      <c r="B80" s="73"/>
       <c r="C80" s="7"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
@@ -8171,10 +8171,10 @@
       <c r="K80" s="3"/>
     </row>
     <row r="81" spans="1:11" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="70" t="s">
+      <c r="A81" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="70" t="str">
+      <c r="B81" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A81, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Application Hardening</v>
       </c>
@@ -8201,8 +8201,8 @@
       <c r="K81" s="3"/>
     </row>
     <row r="82" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="71"/>
-      <c r="B82" s="71"/>
+      <c r="A82" s="73"/>
+      <c r="B82" s="73"/>
       <c r="C82" s="7"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
@@ -8214,10 +8214,10 @@
       <c r="K82" s="3"/>
     </row>
     <row r="83" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="70" t="s">
+      <c r="A83" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="70" t="str">
+      <c r="B83" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A83, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Environment Security Logging</v>
       </c>
@@ -8244,8 +8244,8 @@
       <c r="K83" s="3"/>
     </row>
     <row r="84" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="71"/>
-      <c r="B84" s="71"/>
+      <c r="A84" s="73"/>
+      <c r="B84" s="73"/>
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
       <c r="E84" s="6"/>
@@ -8257,10 +8257,10 @@
       <c r="K84" s="3"/>
     </row>
     <row r="85" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="70" t="s">
+      <c r="A85" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="B85" s="70" t="str">
+      <c r="B85" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A85, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Application Security Logging</v>
       </c>
@@ -8287,8 +8287,8 @@
       <c r="K85" s="3"/>
     </row>
     <row r="86" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="71"/>
-      <c r="B86" s="71"/>
+      <c r="A86" s="73"/>
+      <c r="B86" s="73"/>
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
       <c r="E86" s="6"/>
@@ -8300,10 +8300,10 @@
       <c r="K86" s="3"/>
     </row>
     <row r="87" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="70" t="s">
+      <c r="A87" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="B87" s="70" t="str">
+      <c r="B87" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A87, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Vulnerability Disclosure</v>
       </c>
@@ -8330,8 +8330,8 @@
       <c r="K87" s="3"/>
     </row>
     <row r="88" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="71"/>
-      <c r="B88" s="71"/>
+      <c r="A88" s="73"/>
+      <c r="B88" s="73"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="6"/>
@@ -8343,10 +8343,10 @@
       <c r="K88" s="3"/>
     </row>
     <row r="89" spans="1:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="70" t="s">
+      <c r="A89" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="B89" s="70" t="str">
+      <c r="B89" s="72" t="str">
         <f>VLOOKUP(CONCATENATE($A89, "-", B$1),LevelDescription,2,FALSE)</f>
         <v>Certificate Management</v>
       </c>
@@ -8373,8 +8373,8 @@
       <c r="K89" s="3"/>
     </row>
     <row r="90" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="71"/>
-      <c r="B90" s="71"/>
+      <c r="A90" s="73"/>
+      <c r="B90" s="73"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -20269,47 +20269,32 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A65:A66"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -20326,32 +20311,47 @@
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
@@ -20500,7 +20500,7 @@
       <c r="H10" s="95"/>
       <c r="I10" s="95"/>
     </row>
-    <row r="11" spans="1:9" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>114</v>
       </c>
@@ -20572,7 +20572,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>116</v>
       </c>
@@ -20608,7 +20608,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>117</v>
       </c>
@@ -20644,7 +20644,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>7</v>
       </c>
@@ -20680,7 +20680,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>9</v>
       </c>
@@ -20752,7 +20752,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>14</v>
       </c>
@@ -20788,7 +20788,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>20</v>
       </c>
@@ -20824,7 +20824,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
         <v>111</v>
       </c>
@@ -20860,7 +20860,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>26</v>
       </c>
@@ -20896,7 +20896,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
         <v>29</v>
       </c>
@@ -21004,7 +21004,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
         <v>41</v>
       </c>
@@ -21040,7 +21040,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
         <v>44</v>
       </c>
@@ -21076,7 +21076,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
         <v>46</v>
       </c>
@@ -21148,7 +21148,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>141</v>
       </c>
@@ -21184,7 +21184,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>48</v>
       </c>
@@ -21292,7 +21292,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>58</v>
       </c>
@@ -21328,7 +21328,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
         <v>60</v>
       </c>

</xml_diff>